<commit_message>
Fixed axis of map
</commit_message>
<xml_diff>
--- a/lib/Vortex128.xlsx
+++ b/lib/Vortex128.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ayash\Sailproj\SailProjGit\SAILcode\lib\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34B6C2D3-F910-4AE8-B7B7-C9467DABEE1C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72716109-D967-40EB-B653-94C4FF1EB270}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="522" xr2:uid="{93DD1A3E-79F5-40A0-9DE4-B4C0229D9C52}"/>
   </bookViews>
@@ -1254,8 +1254,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7758D255-7225-412E-BCCB-5D6A66A51808}">
   <dimension ref="A2:V43"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1477,8 +1477,8 @@
         <v>2500</v>
       </c>
       <c r="G13" s="18">
-        <f>-(2^10)</f>
-        <v>-1024</v>
+        <f>0</f>
+        <v>0</v>
       </c>
       <c r="H13" s="18">
         <f>2^12</f>
@@ -2461,23 +2461,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="3be8e3c0-2842-4b5c-b060-a331e5ce9465" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010085EDC4FCBFEAC44C90B472F1F1C900EA" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="e45273375250329c822a0a405177b348">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="3be8e3c0-2842-4b5c-b060-a331e5ce9465" xmlns:ns4="6b4e13fc-0909-4af8-88c8-1f82cb55b253" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="a0e1ca657407e685f067414fb59c7721" ns3:_="" ns4:_="">
     <xsd:import namespace="3be8e3c0-2842-4b5c-b060-a331e5ce9465"/>
@@ -2706,32 +2689,24 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5F39B334-7462-4EA1-A1AF-57733766443C}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="3be8e3c0-2842-4b5c-b060-a331e5ce9465"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="6b4e13fc-0909-4af8-88c8-1f82cb55b253"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1B746C5C-9FCE-47B1-9B21-C70DB5E5E0E1}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="3be8e3c0-2842-4b5c-b060-a331e5ce9465" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{917E079B-BC71-4494-9E92-79C803C2F6BC}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2748,4 +2723,29 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1B746C5C-9FCE-47B1-9B21-C70DB5E5E0E1}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5F39B334-7462-4EA1-A1AF-57733766443C}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="3be8e3c0-2842-4b5c-b060-a331e5ce9465"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="6b4e13fc-0909-4af8-88c8-1f82cb55b253"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Cleanup files and implemented multiple plot windiws
</commit_message>
<xml_diff>
--- a/lib/Vortex128.xlsx
+++ b/lib/Vortex128.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ayash\Sailproj\SailProjGit\SAILcode\lib\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ayash\Programming\vortex_parser\lib\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72716109-D967-40EB-B653-94C4FF1EB270}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D72DDF78-8808-4EA9-8D53-1816EA68F055}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="522" xr2:uid="{93DD1A3E-79F5-40A0-9DE4-B4C0229D9C52}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="13995" tabRatio="522" xr2:uid="{93DD1A3E-79F5-40A0-9DE4-B4C0229D9C52}"/>
   </bookViews>
   <sheets>
     <sheet name="Format" sheetId="2" r:id="rId1"/>
@@ -1255,7 +1255,7 @@
   <dimension ref="A2:V43"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2461,6 +2461,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010085EDC4FCBFEAC44C90B472F1F1C900EA" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="e45273375250329c822a0a405177b348">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="3be8e3c0-2842-4b5c-b060-a331e5ce9465" xmlns:ns4="6b4e13fc-0909-4af8-88c8-1f82cb55b253" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="a0e1ca657407e685f067414fb59c7721" ns3:_="" ns4:_="">
     <xsd:import namespace="3be8e3c0-2842-4b5c-b060-a331e5ce9465"/>
@@ -2689,15 +2698,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -2707,6 +2707,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1B746C5C-9FCE-47B1-9B21-C70DB5E5E0E1}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{917E079B-BC71-4494-9E92-79C803C2F6BC}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2721,14 +2729,6 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1B746C5C-9FCE-47B1-9B21-C70DB5E5E0E1}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>